<commit_message>
Reviewed CYRS & HSI
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PO3_DGW_PP.xlsx
+++ b/SW deliveries log/PO3_DGW_PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F98050-9315-42CD-AE25-50956AD2BE44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43DC95-E6FB-4F82-8D6F-4837AE4D10F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CF37E19-25A2-4CED-AE59-D4BDD2575E03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -351,35 +351,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -902,7 +902,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -990,7 +990,7 @@
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="14" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -1020,7 +1020,7 @@
       <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1070,10 +1070,13 @@
       <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="F7" s="6">
+        <v>43923</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="I7" s="15"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1098,7 +1101,7 @@
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="15"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1108,20 +1111,23 @@
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="6">
         <v>43892</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="6">
         <v>43923</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="6">
         <v>43892</v>
       </c>
+      <c r="F9" s="6">
+        <v>43923</v>
+      </c>
       <c r="G9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="K9" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1130,20 +1136,23 @@
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="6">
         <v>43923</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="6">
         <v>43923</v>
       </c>
+      <c r="E10" s="6">
+        <v>43953</v>
+      </c>
+      <c r="F10" s="6">
+        <v>43953</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="K10" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -1152,10 +1161,10 @@
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="6">
         <v>43923</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="6">
         <v>43953</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1164,8 +1173,8 @@
       <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="K11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1174,10 +1183,10 @@
       <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="6">
         <v>43953</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="6">
         <v>43953</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1186,8 +1195,8 @@
       <c r="H12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="K12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1196,10 +1205,10 @@
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="6">
         <v>43984</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="6">
         <v>43984</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -1209,7 +1218,7 @@
         <v>40</v>
       </c>
       <c r="I13" s="16"/>
-      <c r="K13" s="15"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated PP with new tasks
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PO3_DGW_PP.xlsx
+++ b/SW deliveries log/PO3_DGW_PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527FA921-8A4A-4C6A-8606-0F0C49B674D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2943BE33-9B83-4604-B404-E472F1ADC326}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CF37E19-25A2-4CED-AE59-D4BDD2575E03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Task</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>24/1/2020</t>
-  </si>
-  <si>
-    <t>Initiation Phase</t>
   </si>
   <si>
     <t>Author: Mariam El-Shakafi</t>
@@ -196,6 +193,84 @@
   </si>
   <si>
     <t>Use SRS V0.6, and CYRS V0.4 to update RTM.</t>
+  </si>
+  <si>
+    <t>CYRS Update</t>
+  </si>
+  <si>
+    <t>Use SIQ sheet answers to modify false requirements in CYRS document.</t>
+  </si>
+  <si>
+    <t>22/2/2020</t>
+  </si>
+  <si>
+    <t>23/2/2020</t>
+  </si>
+  <si>
+    <t>Waiting for SIQ sheet answers</t>
+  </si>
+  <si>
+    <t>21/2/2020</t>
+  </si>
+  <si>
+    <t>SRS Update</t>
+  </si>
+  <si>
+    <t>Use updated CYRS to modify SRS</t>
+  </si>
+  <si>
+    <t>Waiting for CYRS update</t>
+  </si>
+  <si>
+    <t>CYRS &amp; SRS Review</t>
+  </si>
+  <si>
+    <t>1. Create a review sheet for CYRS
+2. Create a review sheet for SRS
+3. Make sure both documents are compatible with SIQ answers</t>
+  </si>
+  <si>
+    <t>Waiting for both documents</t>
+  </si>
+  <si>
+    <t>GDD Creation</t>
+  </si>
+  <si>
+    <t>Basem</t>
+  </si>
+  <si>
+    <t>Use final SRS version to create GDD</t>
+  </si>
+  <si>
+    <t>24/2/2020</t>
+  </si>
+  <si>
+    <t>26/2/2020</t>
+  </si>
+  <si>
+    <t>GDD Review</t>
+  </si>
+  <si>
+    <t>1. Make sure GDD is compatible with SRS
+2. Create a review sheet for GDD</t>
+  </si>
+  <si>
+    <t>GDD Update</t>
+  </si>
+  <si>
+    <t>Use both T.Sharaby's review sheet and Mohamed's review sheet to update GDD</t>
+  </si>
+  <si>
+    <t>27/2/2020</t>
+  </si>
+  <si>
+    <t>Add GDD column to RTM</t>
+  </si>
+  <si>
+    <t>Design Phase</t>
+  </si>
+  <si>
+    <t>Definition Phase</t>
   </si>
 </sst>
 </file>
@@ -242,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,8 +336,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -367,9 +448,31 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="dotted">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -378,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -431,7 +534,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -971,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77CBEE5-836F-4E68-99E7-88FE062854C8}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -989,7 +1098,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1002,7 +1111,7 @@
     </row>
     <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1018,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
@@ -1047,10 +1156,10 @@
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -1065,13 +1174,13 @@
         <v>20</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>15</v>
@@ -1080,10 +1189,10 @@
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -1111,10 +1220,10 @@
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -1126,10 +1235,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>4</v>
@@ -1145,7 +1254,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -1157,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="6">
         <v>43923</v>
@@ -1173,7 +1282,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -1185,10 +1294,10 @@
         <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>4</v>
@@ -1198,13 +1307,13 @@
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6">
         <v>43892</v>
@@ -1226,10 +1335,10 @@
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
@@ -1254,13 +1363,13 @@
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="6">
         <v>43923</v>
@@ -1272,7 +1381,7 @@
         <v>43984</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1282,13 +1391,13 @@
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D12" s="6">
         <v>43953</v>
@@ -1297,10 +1406,10 @@
         <v>43953</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>4</v>
@@ -1310,25 +1419,25 @@
     </row>
     <row r="13" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>4</v>
@@ -1338,84 +1447,224 @@
     </row>
     <row r="14" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="17"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
+      <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8"/>
     </row>
-    <row r="30" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
     </row>
     <row r="33" spans="2:2" s="3" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1437,10 +1686,11 @@
       <c r="B38" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J4:J14"/>
+    <mergeCell ref="J4:J17"/>
+    <mergeCell ref="J18:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H86">
     <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Problems">
@@ -1456,7 +1706,7 @@
       <formula>NOT(ISERROR(SEARCH("Not started",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Choose from the drop-down list" sqref="H4:H38" xr:uid="{F112ACAC-A447-4858-94FC-F76DDB174C38}">
       <formula1>$K$3:$K$6</formula1>
     </dataValidation>

</xml_diff>